<commit_message>
pls ignore , submit code to sync up local v.s github.com
</commit_message>
<xml_diff>
--- a/test_calculation/Assumption.xlsx
+++ b/test_calculation/Assumption.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\changer\engine\test_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED2A8DF6-708F-414A-B911-0ED6AF23D8B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C1BA2-288D-4E02-8EE1-821122E2CA0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2110" yWindow="0" windowWidth="15660" windowHeight="10800" xr2:uid="{91C9FA84-EA84-4501-89C0-E757AE774EEC}"/>
+    <workbookView xWindow="-12120" yWindow="4785" windowWidth="28800" windowHeight="15765" xr2:uid="{91C9FA84-EA84-4501-89C0-E757AE774EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>SMM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -49,6 +48,38 @@
   </si>
   <si>
     <t>CPR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tApplyPoolAssump</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yearly cdr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>daily def rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>days</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>observe date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>projected</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -73,12 +104,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -95,11 +132,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -416,112 +456,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B68C88-DA4A-4131-9796-6DF23959880E}">
-  <dimension ref="B1:G12"/>
+  <dimension ref="A2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="1">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="1">
         <v>43101</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>0.01</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="1">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="1">
         <v>43160</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>0.02</v>
       </c>
-      <c r="F4">
-        <f>(B4-B3)/30</f>
+      <c r="F5">
+        <f>(B5-B4)/30</f>
         <v>1.9666666666666666</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F5">
-        <f>F4*C3</f>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <f>F5*C4</f>
         <v>1.9666666666666666E-2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="1">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="1">
         <v>43101</v>
       </c>
-      <c r="C10">
+      <c r="C11">
         <v>0.03</v>
       </c>
-      <c r="F10">
+      <c r="F11">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="1">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
         <v>43160</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>0.05</v>
       </c>
-      <c r="F11">
-        <f>(B11-B10)/365</f>
+      <c r="F12">
+        <f>(B12-B11)/365</f>
         <v>0.16164383561643836</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="F12">
-        <f>F11*C10</f>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <f>F12*C11</f>
         <v>4.8493150684931503E-3</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G13" t="s">
         <v>4</v>
       </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B18" s="1">
+        <v>43132</v>
+      </c>
+      <c r="C18">
+        <v>0.03</v>
+      </c>
+      <c r="D18">
+        <f>1-POWER((1-C18),1/365)</f>
+        <v>8.3446401675124626E-5</v>
+      </c>
+      <c r="E18">
+        <f>B18-A18</f>
+        <v>31</v>
+      </c>
+      <c r="F18">
+        <f>E18*D18</f>
+        <v>2.5868384519288634E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <f>B18</f>
+        <v>43132</v>
+      </c>
+      <c r="B19" s="1">
+        <v>43160</v>
+      </c>
+      <c r="C19">
+        <v>0.04</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ref="D19:D20" si="0">1-POWER((1-C19),1/365)</f>
+        <v>1.1183482689691715E-4</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ref="E19:E20" si="1">B19-B18</f>
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ref="F19:F20" si="2">E19*D19</f>
+        <v>3.1313751531136802E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <f>B19</f>
+        <v>43160</v>
+      </c>
+      <c r="B20" s="1">
+        <v>43191</v>
+      </c>
+      <c r="C20">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1.2613982041997929E-4</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>3.9103344330193579E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1">
+        <v>43110</v>
+      </c>
+      <c r="C24" s="2">
+        <f>C18</f>
+        <v>0.03</v>
+      </c>
+      <c r="D24" s="2">
+        <f>D18</f>
+        <v>8.3446401675124626E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>43141</v>
+      </c>
+      <c r="C25" s="2">
+        <f>C19</f>
+        <v>0.04</v>
+      </c>
+      <c r="D25" s="2">
+        <f>D19</f>
+        <v>1.1183482689691715E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>43156</v>
+      </c>
+      <c r="C26" s="2">
+        <f>C19</f>
+        <v>0.04</v>
+      </c>
+      <c r="D26" s="2">
+        <f>D19</f>
+        <v>1.1183482689691715E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>43110</v>
+      </c>
+      <c r="C29" s="1">
+        <f>B30-1</f>
+        <v>43131</v>
+      </c>
+      <c r="D29">
+        <f>D24</f>
+        <v>8.3446401675124626E-5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>43132</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" ref="C30:C33" si="3">B31-1</f>
+        <v>43140</v>
+      </c>
+      <c r="D30">
+        <f>D19</f>
+        <v>1.1183482689691715E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="1">
+        <v>43141</v>
+      </c>
+      <c r="C31" s="1">
+        <f t="shared" si="3"/>
+        <v>43155</v>
+      </c>
+      <c r="D31">
+        <f>D19</f>
+        <v>1.1183482689691715E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="1">
+        <f>B26</f>
+        <v>43156</v>
+      </c>
+      <c r="C32" s="1">
+        <f t="shared" si="3"/>
+        <v>43159</v>
+      </c>
+      <c r="D32">
+        <f>D19</f>
+        <v>1.1183482689691715E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="1">
+        <v>43160</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Add : prorata util function
</commit_message>
<xml_diff>
--- a/test_calculation/Assumption.xlsx
+++ b/test_calculation/Assumption.xlsx
@@ -1,31 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\changer\engine\test_calculation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771C1BA2-288D-4E02-8EE1-821122E2CA0B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF263215-E4A8-419A-8001-B9CBF3ADC78A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12120" yWindow="4785" windowWidth="28800" windowHeight="15765" xr2:uid="{91C9FA84-EA84-4501-89C0-E757AE774EEC}"/>
+    <workbookView minimized="1" xWindow="640" yWindow="640" windowWidth="16210" windowHeight="9880" xr2:uid="{91C9FA84-EA84-4501-89C0-E757AE774EEC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="UnitTest" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>SMM</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,6 +87,17 @@
   </si>
   <si>
     <t>projected</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rAssumption</t>
+  </si>
+  <si>
+    <t>Proj Dates</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>day-rate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -87,7 +105,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +124,18 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -132,7 +169,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -140,6 +177,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -455,10 +504,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEF44C2-EB11-4613-AA6B-F8B86F62D47D}">
+  <dimension ref="A2:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="6" max="7" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43101</v>
+      </c>
+      <c r="B4" s="1">
+        <f>A5-1</f>
+        <v>43131</v>
+      </c>
+      <c r="C4" s="3">
+        <f>B4-A4</f>
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="4">
+        <v>43115</v>
+      </c>
+      <c r="G4" s="1">
+        <f>B4</f>
+        <v>43131</v>
+      </c>
+      <c r="H4" s="3">
+        <f>G4-F4</f>
+        <v>16</v>
+      </c>
+      <c r="I4" s="5">
+        <f>H4*D4</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43132</v>
+      </c>
+      <c r="B5" s="1">
+        <v>43160</v>
+      </c>
+      <c r="C5" s="3">
+        <f>B5-A5</f>
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>A5</f>
+        <v>43132</v>
+      </c>
+      <c r="G5" s="4">
+        <v>43146</v>
+      </c>
+      <c r="H5" s="3">
+        <f>G5-F5</f>
+        <v>14</v>
+      </c>
+      <c r="I5" s="5">
+        <f>H5*D5</f>
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58B68C88-DA4A-4131-9796-6DF23959880E}">
   <dimension ref="A2:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -726,7 +882,7 @@
         <v>43132</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" ref="C30:C33" si="3">B31-1</f>
+        <f t="shared" ref="C30:C32" si="3">B31-1</f>
         <v>43140</v>
       </c>
       <c r="D30">

</xml_diff>